<commit_message>
Added Imms recommendations to xlsx and csv with new headers for AB#10856
</commit_message>
<xml_diff>
--- a/Apps/WebClient/src/Server/Assets/Templates/ImmunizationReport.xlsx
+++ b/Apps/WebClient/src/Server/Assets/Templates/ImmunizationReport.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laws/Projects/Health/healthgateway/Apps/WebClient/src/Server/Assets/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC490EF0-258A-1C4A-B59B-C40622468B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8686D28-E2DB-C243-BECB-735B0E340133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5820" yWindow="4960" windowWidth="28040" windowHeight="17440" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Immunizations" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -89,13 +89,43 @@
   </si>
   <si>
     <t>{d.records[i+1].provider_clinic}</t>
+  </si>
+  <si>
+    <t>Immunization History</t>
+  </si>
+  <si>
+    <t>{d.recommendations[i].immunization}</t>
+  </si>
+  <si>
+    <t>{d.recommendations[i+1].immunization}</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>{d.recommendations[i+1].due_date}</t>
+  </si>
+  <si>
+    <t>{d.recommendations[i].status}</t>
+  </si>
+  <si>
+    <t>{d.recommendations[i+1].status}</t>
+  </si>
+  <si>
+    <t>{d.recommendations[i].due_date}</t>
+  </si>
+  <si>
+    <t>Immunization Recommendations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,6 +145,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF606060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,13 +178,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60882D5E-E61D-5940-8D5B-09478E4A9588}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -474,67 +513,110 @@
     <col min="9" max="9" width="44.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Imms recommendations to xlsx and csv with new headers for AB#10856 (#2552)
</commit_message>
<xml_diff>
--- a/Apps/WebClient/src/Server/Assets/Templates/ImmunizationReport.xlsx
+++ b/Apps/WebClient/src/Server/Assets/Templates/ImmunizationReport.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laws/Projects/Health/healthgateway/Apps/WebClient/src/Server/Assets/Templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC490EF0-258A-1C4A-B59B-C40622468B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8686D28-E2DB-C243-BECB-735B0E340133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5820" yWindow="4960" windowWidth="28040" windowHeight="17440" xr2:uid="{F605F369-0C71-414E-B75C-5C18C8076E19}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Immunizations" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -89,13 +89,43 @@
   </si>
   <si>
     <t>{d.records[i+1].provider_clinic}</t>
+  </si>
+  <si>
+    <t>Immunization History</t>
+  </si>
+  <si>
+    <t>{d.recommendations[i].immunization}</t>
+  </si>
+  <si>
+    <t>{d.recommendations[i+1].immunization}</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>{d.recommendations[i+1].due_date}</t>
+  </si>
+  <si>
+    <t>{d.recommendations[i].status}</t>
+  </si>
+  <si>
+    <t>{d.recommendations[i+1].status}</t>
+  </si>
+  <si>
+    <t>{d.recommendations[i].due_date}</t>
+  </si>
+  <si>
+    <t>Immunization Recommendations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,6 +145,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF606060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,13 +178,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,7 +500,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60882D5E-E61D-5940-8D5B-09478E4A9588}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -474,67 +513,110 @@
     <col min="9" max="9" width="44.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>